<commit_message>
Inc. face detection accurracy
</commit_message>
<xml_diff>
--- a/entries.xlsx
+++ b/entries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -417,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -812,7 +812,79 @@
         <v>11</v>
       </c>
       <c r="B49" s="2">
-        <v>44708.07832020292</v>
+        <v>44708.07832020833</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="2">
+        <v>44708.70932243056</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="2">
+        <v>44708.70997974537</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="2">
+        <v>44708.73424809028</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="2">
+        <v>44708.73463961806</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="2">
+        <v>44708.74323366898</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="2">
+        <v>44709.00327535879</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="2">
+        <v>44709.00349340278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="2">
+        <v>44709.00361327546</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="2">
+        <v>44709.01079778255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>